<commit_message>
modified:   decimalodd.ipynb 	modified:   decimalodd_res/bb.xlsx 	modified:   decimalodd_res/macd.xlsx 	modified:   decimalodd_res/obv.xlsx 	modified:   winrate_result/bb.xlsx 	modified:   winrate_result/macd.xlsx 	modified:   winrate_result/obv.xlsx
</commit_message>
<xml_diff>
--- a/decimalodd_res/macd.xlsx
+++ b/decimalodd_res/macd.xlsx
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11967.45417404175</v>
+        <v>119694.7937469482</v>
       </c>
       <c r="D2" t="n">
-        <v>1967.454174041748</v>
+        <v>19694.79374694824</v>
       </c>
       <c r="E2" t="n">
-        <v>19.67454174041748</v>
+        <v>19.69479374694824</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12295.74040222168</v>
+        <v>123477.6673431396</v>
       </c>
       <c r="D3" t="n">
-        <v>2295.74040222168</v>
+        <v>23477.66734313965</v>
       </c>
       <c r="E3" t="n">
-        <v>22.9574040222168</v>
+        <v>23.47766734313965</v>
       </c>
     </row>
     <row r="4">
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11093.76484680176</v>
+        <v>110926.5220222473</v>
       </c>
       <c r="D4" t="n">
-        <v>1093.764846801758</v>
+        <v>10926.52202224731</v>
       </c>
       <c r="E4" t="n">
-        <v>10.93764846801758</v>
+        <v>10.92652202224732</v>
       </c>
     </row>
     <row r="5">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10020.85015869141</v>
+        <v>100226.2015991211</v>
       </c>
       <c r="D5" t="n">
-        <v>20.85015869140625</v>
+        <v>226.2015991210938</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2085015869140625</v>
+        <v>0.2262015991210937</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>11198.47570800781</v>
+        <v>111900.5071563721</v>
       </c>
       <c r="D6" t="n">
-        <v>1198.475708007812</v>
+        <v>11900.50715637207</v>
       </c>
       <c r="E6" t="n">
-        <v>11.98475708007813</v>
+        <v>11.90050715637207</v>
       </c>
     </row>
     <row r="7">
@@ -560,13 +560,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11559.36622619629</v>
+        <v>115734.2852783203</v>
       </c>
       <c r="D7" t="n">
-        <v>1559.366226196289</v>
+        <v>15734.28527832031</v>
       </c>
       <c r="E7" t="n">
-        <v>15.59366226196289</v>
+        <v>15.73428527832031</v>
       </c>
     </row>
     <row r="8">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10670.45517349243</v>
+        <v>106710.4298629761</v>
       </c>
       <c r="D8" t="n">
-        <v>670.4551734924316</v>
+        <v>6710.429862976074</v>
       </c>
       <c r="E8" t="n">
-        <v>6.704551734924316</v>
+        <v>6.710429862976073</v>
       </c>
     </row>
     <row r="9">
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11291.77443695068</v>
+        <v>112959.9247589111</v>
       </c>
       <c r="D9" t="n">
-        <v>1291.774436950684</v>
+        <v>12959.92475891113</v>
       </c>
       <c r="E9" t="n">
-        <v>12.91774436950684</v>
+        <v>12.95992475891113</v>
       </c>
     </row>
     <row r="10">
@@ -617,13 +617,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>12325.7951965332</v>
+        <v>123259.4151859283</v>
       </c>
       <c r="D10" t="n">
-        <v>2325.795196533203</v>
+        <v>23259.41518592834</v>
       </c>
       <c r="E10" t="n">
-        <v>23.25795196533203</v>
+        <v>23.25941518592834</v>
       </c>
     </row>
     <row r="11">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10102.81625366211</v>
+        <v>101058.291595459</v>
       </c>
       <c r="D11" t="n">
-        <v>102.8162536621094</v>
+        <v>1058.291595458984</v>
       </c>
       <c r="E11" t="n">
-        <v>1.028162536621094</v>
+        <v>1.058291595458984</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10045.34897232056</v>
+        <v>100437.4589424133</v>
       </c>
       <c r="D12" t="n">
-        <v>45.34897232055664</v>
+        <v>437.4589424133301</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4534897232055664</v>
+        <v>0.4374589424133301</v>
       </c>
     </row>
     <row r="13">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10846.88224029541</v>
+        <v>108449.3448524475</v>
       </c>
       <c r="D13" t="n">
-        <v>846.8822402954102</v>
+        <v>8449.34485244751</v>
       </c>
       <c r="E13" t="n">
-        <v>8.468822402954101</v>
+        <v>8.44934485244751</v>
       </c>
     </row>
     <row r="14">
@@ -693,13 +693,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>11489.48704147339</v>
+        <v>114942.1506690979</v>
       </c>
       <c r="D14" t="n">
-        <v>1489.487041473389</v>
+        <v>14942.1506690979</v>
       </c>
       <c r="E14" t="n">
-        <v>14.89487041473389</v>
+        <v>14.9421506690979</v>
       </c>
     </row>
     <row r="15">
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>11373.23569488525</v>
+        <v>113758.5279846191</v>
       </c>
       <c r="D15" t="n">
-        <v>1373.235694885254</v>
+        <v>13758.52798461914</v>
       </c>
       <c r="E15" t="n">
-        <v>13.73235694885254</v>
+        <v>13.75852798461914</v>
       </c>
     </row>
     <row r="16">
@@ -731,13 +731,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8898.746269226074</v>
+        <v>88971.87142181396</v>
       </c>
       <c r="D16" t="n">
-        <v>-1101.253730773926</v>
+        <v>-11028.12857818604</v>
       </c>
       <c r="E16" t="n">
-        <v>-11.01253730773926</v>
+        <v>-11.02812857818603</v>
       </c>
     </row>
     <row r="17">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>12014.32466888428</v>
+        <v>120207.0395202637</v>
       </c>
       <c r="D17" t="n">
-        <v>2014.324668884277</v>
+        <v>20207.03952026367</v>
       </c>
       <c r="E17" t="n">
-        <v>20.14324668884277</v>
+        <v>20.20703952026367</v>
       </c>
     </row>
     <row r="18">
@@ -769,13 +769,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12648.40647888184</v>
+        <v>126553.3456268311</v>
       </c>
       <c r="D18" t="n">
-        <v>2648.406478881836</v>
+        <v>26553.34562683105</v>
       </c>
       <c r="E18" t="n">
-        <v>26.48406478881836</v>
+        <v>26.55334562683105</v>
       </c>
     </row>
     <row r="19">
@@ -788,13 +788,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>12588.36934661865</v>
+        <v>123715.6070022583</v>
       </c>
       <c r="D19" t="n">
-        <v>2588.369346618652</v>
+        <v>23715.6070022583</v>
       </c>
       <c r="E19" t="n">
-        <v>25.88369346618653</v>
+        <v>23.7156070022583</v>
       </c>
     </row>
     <row r="20">
@@ -807,13 +807,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8303.514421463013</v>
+        <v>83014.82019805908</v>
       </c>
       <c r="D20" t="n">
-        <v>-1696.485578536987</v>
+        <v>-16985.17980194092</v>
       </c>
       <c r="E20" t="n">
-        <v>-16.96485578536987</v>
+        <v>-16.98517980194092</v>
       </c>
     </row>
     <row r="21">
@@ -826,13 +826,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9168.15213394165</v>
+        <v>91663.25539779663</v>
       </c>
       <c r="D21" t="n">
-        <v>-831.8478660583496</v>
+        <v>-8336.744602203369</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.318478660583496</v>
+        <v>-8.336744602203369</v>
       </c>
     </row>
     <row r="22">
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>12868.80702209473</v>
+        <v>128907.0210113525</v>
       </c>
       <c r="D22" t="n">
-        <v>2868.807022094727</v>
+        <v>28907.02101135254</v>
       </c>
       <c r="E22" t="n">
-        <v>28.68807022094726</v>
+        <v>28.90702101135254</v>
       </c>
     </row>
     <row r="23">
@@ -864,13 +864,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>10480.79203796387</v>
+        <v>104806.0463562012</v>
       </c>
       <c r="D23" t="n">
-        <v>480.7920379638672</v>
+        <v>4806.046356201172</v>
       </c>
       <c r="E23" t="n">
-        <v>4.807920379638672</v>
+        <v>4.806046356201172</v>
       </c>
     </row>
     <row r="24">
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9241.43452835083</v>
+        <v>92416.45233535767</v>
       </c>
       <c r="D24" t="n">
-        <v>-758.5654716491699</v>
+        <v>-7583.547664642334</v>
       </c>
       <c r="E24" t="n">
-        <v>-7.5856547164917</v>
+        <v>-7.583547664642334</v>
       </c>
     </row>
     <row r="25">
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12788.7216796875</v>
+        <v>127995.5507202148</v>
       </c>
       <c r="D25" t="n">
-        <v>2788.7216796875</v>
+        <v>27995.55072021484</v>
       </c>
       <c r="E25" t="n">
-        <v>27.887216796875</v>
+        <v>27.99555072021484</v>
       </c>
     </row>
     <row r="26">
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>11412.91380310059</v>
+        <v>114213.0182418823</v>
       </c>
       <c r="D26" t="n">
-        <v>1412.913803100586</v>
+        <v>14213.01824188232</v>
       </c>
       <c r="E26" t="n">
-        <v>14.12913803100586</v>
+        <v>14.21301824188232</v>
       </c>
     </row>
     <row r="27">
@@ -940,13 +940,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>11526.11618041992</v>
+        <v>115368.2472991943</v>
       </c>
       <c r="D27" t="n">
-        <v>1526.116180419922</v>
+        <v>15368.24729919434</v>
       </c>
       <c r="E27" t="n">
-        <v>15.26116180419922</v>
+        <v>15.36824729919434</v>
       </c>
     </row>
     <row r="28">
@@ -959,13 +959,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>11405.80366516113</v>
+        <v>114075.2806625366</v>
       </c>
       <c r="D28" t="n">
-        <v>1405.803665161133</v>
+        <v>14075.28066253662</v>
       </c>
       <c r="E28" t="n">
-        <v>14.05803665161133</v>
+        <v>14.07528066253662</v>
       </c>
     </row>
     <row r="29">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>13582.169921875</v>
+        <v>136048.807800293</v>
       </c>
       <c r="D29" t="n">
-        <v>3582.169921875</v>
+        <v>36048.80780029297</v>
       </c>
       <c r="E29" t="n">
-        <v>35.82169921875001</v>
+        <v>36.04880780029297</v>
       </c>
     </row>
     <row r="30">
@@ -997,13 +997,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8659.621246337891</v>
+        <v>86550.58252716064</v>
       </c>
       <c r="D30" t="n">
-        <v>-1340.378753662109</v>
+        <v>-13449.41747283936</v>
       </c>
       <c r="E30" t="n">
-        <v>-13.4037875366211</v>
+        <v>-13.44941747283936</v>
       </c>
     </row>
     <row r="31">
@@ -1016,13 +1016,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>10113.61560821533</v>
+        <v>101103.3532676697</v>
       </c>
       <c r="D31" t="n">
-        <v>113.615608215332</v>
+        <v>1103.353267669678</v>
       </c>
       <c r="E31" t="n">
-        <v>1.13615608215332</v>
+        <v>1.103353267669678</v>
       </c>
     </row>
     <row r="32">
@@ -1035,13 +1035,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12351.45983886719</v>
+        <v>124201.0783081055</v>
       </c>
       <c r="D32" t="n">
-        <v>2351.459838867188</v>
+        <v>24201.07830810547</v>
       </c>
       <c r="E32" t="n">
-        <v>23.51459838867187</v>
+        <v>24.20107830810547</v>
       </c>
     </row>
     <row r="33">
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>10276.86791992188</v>
+        <v>102812.4024772644</v>
       </c>
       <c r="D33" t="n">
-        <v>276.867919921875</v>
+        <v>2812.402477264404</v>
       </c>
       <c r="E33" t="n">
-        <v>2.76867919921875</v>
+        <v>2.812402477264405</v>
       </c>
     </row>
     <row r="34">
@@ -1073,13 +1073,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>7915.866851806641</v>
+        <v>79094.5196685791</v>
       </c>
       <c r="D34" t="n">
-        <v>-2084.133148193359</v>
+        <v>-20905.4803314209</v>
       </c>
       <c r="E34" t="n">
-        <v>-20.84133148193359</v>
+        <v>-20.9054803314209</v>
       </c>
     </row>
     <row r="35">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>14097.01382446289</v>
+        <v>141016.3170471191</v>
       </c>
       <c r="D35" t="n">
-        <v>4097.013824462891</v>
+        <v>41016.31704711914</v>
       </c>
       <c r="E35" t="n">
-        <v>40.97013824462891</v>
+        <v>41.01631704711914</v>
       </c>
     </row>
     <row r="36">
@@ -1111,13 +1111,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>10433.96601104736</v>
+        <v>104317.9474334717</v>
       </c>
       <c r="D36" t="n">
-        <v>433.9660110473633</v>
+        <v>4317.94743347168</v>
       </c>
       <c r="E36" t="n">
-        <v>4.339660110473633</v>
+        <v>4.31794743347168</v>
       </c>
     </row>
     <row r="37">
@@ -1130,13 +1130,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>9687.243804931641</v>
+        <v>96889.24454116821</v>
       </c>
       <c r="D37" t="n">
-        <v>-312.7561950683594</v>
+        <v>-3110.755458831787</v>
       </c>
       <c r="E37" t="n">
-        <v>-3.127561950683594</v>
+        <v>-3.110755458831787</v>
       </c>
     </row>
     <row r="38">
@@ -1149,13 +1149,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>14764.5908203125</v>
+        <v>148272.2018432617</v>
       </c>
       <c r="D38" t="n">
-        <v>4764.5908203125</v>
+        <v>48272.20184326172</v>
       </c>
       <c r="E38" t="n">
-        <v>47.645908203125</v>
+        <v>48.27220184326172</v>
       </c>
     </row>
     <row r="39">
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>12246.97869873047</v>
+        <v>122907.5224914551</v>
       </c>
       <c r="D39" t="n">
-        <v>2246.978698730469</v>
+        <v>22907.52249145508</v>
       </c>
       <c r="E39" t="n">
-        <v>22.46978698730469</v>
+        <v>22.90752249145508</v>
       </c>
     </row>
     <row r="40">
@@ -1187,13 +1187,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>12926.22383117676</v>
+        <v>129383.3076782227</v>
       </c>
       <c r="D40" t="n">
-        <v>2926.223831176758</v>
+        <v>29383.30767822266</v>
       </c>
       <c r="E40" t="n">
-        <v>29.26223831176758</v>
+        <v>29.38330767822266</v>
       </c>
     </row>
     <row r="41">
@@ -1206,13 +1206,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>10571.96692657471</v>
+        <v>105716.2997741699</v>
       </c>
       <c r="D41" t="n">
-        <v>571.966926574707</v>
+        <v>5716.299774169922</v>
       </c>
       <c r="E41" t="n">
-        <v>5.71966926574707</v>
+        <v>5.716299774169921</v>
       </c>
     </row>
     <row r="42">
@@ -1225,13 +1225,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>7295.050717353821</v>
+        <v>72933.78718090057</v>
       </c>
       <c r="D42" t="n">
-        <v>-2704.949282646179</v>
+        <v>-27066.21281909943</v>
       </c>
       <c r="E42" t="n">
-        <v>-27.04949282646179</v>
+        <v>-27.06621281909943</v>
       </c>
     </row>
     <row r="43">
@@ -1244,13 +1244,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>9079.186065673828</v>
+        <v>90677.67463684082</v>
       </c>
       <c r="D43" t="n">
-        <v>-920.8139343261719</v>
+        <v>-9322.32536315918</v>
       </c>
       <c r="E43" t="n">
-        <v>-9.208139343261719</v>
+        <v>-9.32232536315918</v>
       </c>
     </row>
     <row r="44">
@@ -1263,13 +1263,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12139.31243133545</v>
+        <v>121422.9367828369</v>
       </c>
       <c r="D44" t="n">
-        <v>2139.312431335449</v>
+        <v>21422.93678283691</v>
       </c>
       <c r="E44" t="n">
-        <v>21.39312431335449</v>
+        <v>21.42293678283691</v>
       </c>
     </row>
     <row r="45">
@@ -1282,13 +1282,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>10484.74975585938</v>
+        <v>104875.0488052368</v>
       </c>
       <c r="D45" t="n">
-        <v>484.749755859375</v>
+        <v>4875.048805236816</v>
       </c>
       <c r="E45" t="n">
-        <v>4.847497558593751</v>
+        <v>4.875048805236816</v>
       </c>
     </row>
     <row r="46">
@@ -1301,13 +1301,13 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>11435.34292984009</v>
+        <v>114420.8460464478</v>
       </c>
       <c r="D46" t="n">
-        <v>1435.342929840088</v>
+        <v>14420.84604644775</v>
       </c>
       <c r="E46" t="n">
-        <v>14.35342929840088</v>
+        <v>14.42084604644776</v>
       </c>
     </row>
     <row r="47">
@@ -1320,13 +1320,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>10311.14782714844</v>
+        <v>103032.5048675537</v>
       </c>
       <c r="D47" t="n">
-        <v>311.1478271484375</v>
+        <v>3032.504867553711</v>
       </c>
       <c r="E47" t="n">
-        <v>3.111478271484375</v>
+        <v>3.032504867553711</v>
       </c>
     </row>
     <row r="48">
@@ -1339,13 +1339,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>12163.8948135376</v>
+        <v>121722.1455535889</v>
       </c>
       <c r="D48" t="n">
-        <v>2163.894813537598</v>
+        <v>21722.14555358887</v>
       </c>
       <c r="E48" t="n">
-        <v>21.63894813537598</v>
+        <v>21.72214555358887</v>
       </c>
     </row>
     <row r="49">
@@ -1358,13 +1358,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>10829.74482727051</v>
+        <v>108312.7405395508</v>
       </c>
       <c r="D49" t="n">
-        <v>829.7448272705078</v>
+        <v>8312.740539550781</v>
       </c>
       <c r="E49" t="n">
-        <v>8.297448272705079</v>
+        <v>8.312740539550781</v>
       </c>
     </row>
     <row r="50">
@@ -1377,13 +1377,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6487.049720287323</v>
+        <v>64843.09720420837</v>
       </c>
       <c r="D50" t="n">
-        <v>-3512.950279712677</v>
+        <v>-35156.90279579163</v>
       </c>
       <c r="E50" t="n">
-        <v>-35.12950279712677</v>
+        <v>-35.15690279579163</v>
       </c>
     </row>
     <row r="51">
@@ -1396,13 +1396,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>10936.77381896973</v>
+        <v>109380.7565765381</v>
       </c>
       <c r="D51" t="n">
-        <v>936.7738189697266</v>
+        <v>9380.756576538086</v>
       </c>
       <c r="E51" t="n">
-        <v>9.367738189697265</v>
+        <v>9.380756576538086</v>
       </c>
     </row>
     <row r="52">
@@ -1415,13 +1415,13 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6421.018983840942</v>
+        <v>64204.85983586311</v>
       </c>
       <c r="D52" t="n">
-        <v>-3578.981016159058</v>
+        <v>-35795.14016413689</v>
       </c>
       <c r="E52" t="n">
-        <v>-35.78981016159057</v>
+        <v>-35.79514016413688</v>
       </c>
     </row>
     <row r="53">
@@ -1434,13 +1434,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>10346.84575653076</v>
+        <v>103474.6545181274</v>
       </c>
       <c r="D53" t="n">
-        <v>346.8457565307617</v>
+        <v>3474.654518127441</v>
       </c>
       <c r="E53" t="n">
-        <v>3.468457565307617</v>
+        <v>3.474654518127442</v>
       </c>
     </row>
     <row r="54">
@@ -1453,13 +1453,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>10212.64212608337</v>
+        <v>102127.6962070465</v>
       </c>
       <c r="D54" t="n">
-        <v>212.642126083374</v>
+        <v>2127.696207046509</v>
       </c>
       <c r="E54" t="n">
-        <v>2.12642126083374</v>
+        <v>2.127696207046509</v>
       </c>
     </row>
     <row r="55">
@@ -1472,13 +1472,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>9286</v>
+        <v>92933</v>
       </c>
       <c r="D55" t="n">
-        <v>-714</v>
+        <v>-7067</v>
       </c>
       <c r="E55" t="n">
-        <v>-7.140000000000001</v>
+        <v>-7.066999999999999</v>
       </c>
     </row>
     <row r="56">
@@ -1491,13 +1491,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5084.799438476562</v>
+        <v>48780.54443359375</v>
       </c>
       <c r="D56" t="n">
-        <v>-4915.200561523438</v>
+        <v>-51219.45556640625</v>
       </c>
       <c r="E56" t="n">
-        <v>-49.15200561523437</v>
+        <v>-51.21945556640625</v>
       </c>
     </row>
     <row r="57">
@@ -1510,13 +1510,13 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>9527.421646118164</v>
+        <v>95165.48588562012</v>
       </c>
       <c r="D57" t="n">
-        <v>-472.5783538818359</v>
+        <v>-4834.514114379883</v>
       </c>
       <c r="E57" t="n">
-        <v>-4.72578353881836</v>
+        <v>-4.834514114379883</v>
       </c>
     </row>
     <row r="58">
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>11594.43132400513</v>
+        <v>116036.8251304626</v>
       </c>
       <c r="D58" t="n">
-        <v>1594.431324005127</v>
+        <v>16036.82513046265</v>
       </c>
       <c r="E58" t="n">
-        <v>15.94431324005127</v>
+        <v>16.03682513046265</v>
       </c>
     </row>
     <row r="59">
@@ -1548,13 +1548,13 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>8059.371597290039</v>
+        <v>80529.41600799561</v>
       </c>
       <c r="D59" t="n">
-        <v>-1940.628402709961</v>
+        <v>-19470.58399200439</v>
       </c>
       <c r="E59" t="n">
-        <v>-19.40628402709961</v>
+        <v>-19.4705839920044</v>
       </c>
     </row>
     <row r="60">
@@ -1567,13 +1567,13 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>8480.252616882324</v>
+        <v>84781.00667190552</v>
       </c>
       <c r="D60" t="n">
-        <v>-1519.747383117676</v>
+        <v>-15218.99332809448</v>
       </c>
       <c r="E60" t="n">
-        <v>-15.19747383117676</v>
+        <v>-15.21899332809448</v>
       </c>
     </row>
     <row r="61">
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>7760.833671569824</v>
+        <v>77545.27185821533</v>
       </c>
       <c r="D61" t="n">
-        <v>-2239.166328430176</v>
+        <v>-22454.72814178467</v>
       </c>
       <c r="E61" t="n">
-        <v>-22.39166328430176</v>
+        <v>-22.45472814178467</v>
       </c>
     </row>
     <row r="62">
@@ -1605,13 +1605,13 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>6275.079476356506</v>
+        <v>62717.34475803375</v>
       </c>
       <c r="D62" t="n">
-        <v>-3724.920523643494</v>
+        <v>-37282.65524196625</v>
       </c>
       <c r="E62" t="n">
-        <v>-37.24920523643493</v>
+        <v>-37.28265524196625</v>
       </c>
     </row>
     <row r="63">
@@ -1624,13 +1624,13 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>12297.20214080811</v>
+        <v>123034.6314697266</v>
       </c>
       <c r="D63" t="n">
-        <v>2297.202140808105</v>
+        <v>23034.63146972656</v>
       </c>
       <c r="E63" t="n">
-        <v>22.97202140808105</v>
+        <v>23.03463146972656</v>
       </c>
     </row>
     <row r="64">
@@ -1643,13 +1643,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>11864.19421005249</v>
+        <v>118691.3671531677</v>
       </c>
       <c r="D64" t="n">
-        <v>1864.19421005249</v>
+        <v>18691.36715316772</v>
       </c>
       <c r="E64" t="n">
-        <v>18.6419421005249</v>
+        <v>18.69136715316772</v>
       </c>
     </row>
     <row r="65">
@@ -1662,13 +1662,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>16618.45965576172</v>
+        <v>168090.3964538574</v>
       </c>
       <c r="D65" t="n">
-        <v>6618.459655761719</v>
+        <v>68090.39645385742</v>
       </c>
       <c r="E65" t="n">
-        <v>66.1845965576172</v>
+        <v>68.09039645385742</v>
       </c>
     </row>
     <row r="66">
@@ -1681,13 +1681,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>8305.508567810059</v>
+        <v>83036.58343315125</v>
       </c>
       <c r="D66" t="n">
-        <v>-1694.491432189941</v>
+        <v>-16963.41656684875</v>
       </c>
       <c r="E66" t="n">
-        <v>-16.94491432189941</v>
+        <v>-16.96341656684875</v>
       </c>
     </row>
     <row r="67">
@@ -1700,13 +1700,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>12442.85207343102</v>
+        <v>124418.7358617783</v>
       </c>
       <c r="D67" t="n">
-        <v>2442.852073431015</v>
+        <v>24418.73586177826</v>
       </c>
       <c r="E67" t="n">
-        <v>24.42852073431015</v>
+        <v>24.41873586177826</v>
       </c>
     </row>
     <row r="68">
@@ -1719,13 +1719,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>10155.86006045341</v>
+        <v>101554.1206054688</v>
       </c>
       <c r="D68" t="n">
-        <v>155.8600604534149</v>
+        <v>1554.12060546875</v>
       </c>
       <c r="E68" t="n">
-        <v>1.558600604534149</v>
+        <v>1.55412060546875</v>
       </c>
     </row>
     <row r="69">
@@ -1738,13 +1738,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5790.979246139526</v>
+        <v>57869.80146312714</v>
       </c>
       <c r="D69" t="n">
-        <v>-4209.020753860474</v>
+        <v>-42130.19853687286</v>
       </c>
       <c r="E69" t="n">
-        <v>-42.09020753860474</v>
+        <v>-42.13019853687287</v>
       </c>
     </row>
     <row r="70">
@@ -1757,13 +1757,13 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>11680.16821289062</v>
+        <v>116904.8969268799</v>
       </c>
       <c r="D70" t="n">
-        <v>1680.168212890625</v>
+        <v>16904.89692687988</v>
       </c>
       <c r="E70" t="n">
-        <v>16.80168212890625</v>
+        <v>16.90489692687988</v>
       </c>
     </row>
     <row r="71">
@@ -1776,13 +1776,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>14132.00491714478</v>
+        <v>141363.4424552917</v>
       </c>
       <c r="D71" t="n">
-        <v>4132.004917144775</v>
+        <v>41363.44245529175</v>
       </c>
       <c r="E71" t="n">
-        <v>41.32004917144776</v>
+        <v>41.36344245529175</v>
       </c>
     </row>
     <row r="72">
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -1814,13 +1814,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>10643.67098236084</v>
+        <v>106418.5398635864</v>
       </c>
       <c r="D73" t="n">
-        <v>643.6709823608398</v>
+        <v>6418.539863586426</v>
       </c>
       <c r="E73" t="n">
-        <v>6.436709823608398</v>
+        <v>6.418539863586425</v>
       </c>
     </row>
     <row r="74">
@@ -1833,13 +1833,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7662.392935752869</v>
+        <v>76615.62582588196</v>
       </c>
       <c r="D74" t="n">
-        <v>-2337.607064247131</v>
+        <v>-23384.37417411804</v>
       </c>
       <c r="E74" t="n">
-        <v>-23.37607064247131</v>
+        <v>-23.38437417411804</v>
       </c>
     </row>
     <row r="75">
@@ -1852,13 +1852,13 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8005.359952449799</v>
+        <v>80047.51452445984</v>
       </c>
       <c r="D75" t="n">
-        <v>-1994.640047550201</v>
+        <v>-19952.48547554016</v>
       </c>
       <c r="E75" t="n">
-        <v>-19.94640047550201</v>
+        <v>-19.95248547554016</v>
       </c>
     </row>
     <row r="76">
@@ -1871,13 +1871,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>9678.283420085907</v>
+        <v>96778.87296581268</v>
       </c>
       <c r="D76" t="n">
-        <v>-321.716579914093</v>
+        <v>-3221.127034187317</v>
       </c>
       <c r="E76" t="n">
-        <v>-3.21716579914093</v>
+        <v>-3.221127034187317</v>
       </c>
     </row>
     <row r="77">
@@ -1890,13 +1890,13 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>13296.07415771484</v>
+        <v>133297.4388122559</v>
       </c>
       <c r="D77" t="n">
-        <v>3296.074157714844</v>
+        <v>33297.43881225586</v>
       </c>
       <c r="E77" t="n">
-        <v>32.96074157714844</v>
+        <v>33.29743881225586</v>
       </c>
     </row>
     <row r="78">
@@ -1909,13 +1909,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>10619.7798538208</v>
+        <v>106222.1486053467</v>
       </c>
       <c r="D78" t="n">
-        <v>619.7798538208008</v>
+        <v>6222.14860534668</v>
       </c>
       <c r="E78" t="n">
-        <v>6.197798538208008</v>
+        <v>6.22214860534668</v>
       </c>
     </row>
     <row r="79">
@@ -1928,13 +1928,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>15564.59938812256</v>
+        <v>155904.003868103</v>
       </c>
       <c r="D79" t="n">
-        <v>5564.599388122559</v>
+        <v>55904.00386810303</v>
       </c>
       <c r="E79" t="n">
-        <v>55.64599388122559</v>
+        <v>55.90400386810303</v>
       </c>
     </row>
     <row r="80">
@@ -1947,13 +1947,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>3622.779886603355</v>
+        <v>36222.30886530876</v>
       </c>
       <c r="D80" t="n">
-        <v>-6377.220113396645</v>
+        <v>-63777.69113469124</v>
       </c>
       <c r="E80" t="n">
-        <v>-63.77220113396645</v>
+        <v>-63.77769113469124</v>
       </c>
     </row>
     <row r="81">
@@ -1966,13 +1966,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4522.810033798218</v>
+        <v>45210.22033905983</v>
       </c>
       <c r="D81" t="n">
-        <v>-5477.189966201782</v>
+        <v>-54789.77966094017</v>
       </c>
       <c r="E81" t="n">
-        <v>-54.77189966201782</v>
+        <v>-54.78977966094018</v>
       </c>
     </row>
     <row r="82">
@@ -1985,13 +1985,13 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>7784.040148735046</v>
+        <v>77821.57149410248</v>
       </c>
       <c r="D82" t="n">
-        <v>-2215.959851264954</v>
+        <v>-22178.42850589752</v>
       </c>
       <c r="E82" t="n">
-        <v>-22.15959851264954</v>
+        <v>-22.17842850589752</v>
       </c>
     </row>
     <row r="83">
@@ -2004,13 +2004,13 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>5448.150024414062</v>
+        <v>54368.49025154114</v>
       </c>
       <c r="D83" t="n">
-        <v>-4551.849975585938</v>
+        <v>-45631.50974845886</v>
       </c>
       <c r="E83" t="n">
-        <v>-45.51849975585937</v>
+        <v>-45.63150974845887</v>
       </c>
     </row>
     <row r="84">
@@ -2023,13 +2023,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>12146.02588653564</v>
+        <v>121493.9067192078</v>
       </c>
       <c r="D84" t="n">
-        <v>2146.025886535645</v>
+        <v>21493.90671920776</v>
       </c>
       <c r="E84" t="n">
-        <v>21.46025886535645</v>
+        <v>21.49390671920776</v>
       </c>
     </row>
     <row r="85">
@@ -2042,13 +2042,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>9386.749011993408</v>
+        <v>93867.10158157349</v>
       </c>
       <c r="D85" t="n">
-        <v>-613.2509880065918</v>
+        <v>-6132.898418426514</v>
       </c>
       <c r="E85" t="n">
-        <v>-6.132509880065918</v>
+        <v>-6.132898418426514</v>
       </c>
     </row>
     <row r="86">
@@ -2061,13 +2061,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4880.830554962158</v>
+        <v>48698.1255569458</v>
       </c>
       <c r="D86" t="n">
-        <v>-5119.169445037842</v>
+        <v>-51301.8744430542</v>
       </c>
       <c r="E86" t="n">
-        <v>-51.19169445037842</v>
+        <v>-51.3018744430542</v>
       </c>
     </row>
     <row r="87">
@@ -2080,13 +2080,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>10090.60290527344</v>
+        <v>100931.7696228027</v>
       </c>
       <c r="D87" t="n">
-        <v>90.6029052734375</v>
+        <v>931.7696228027344</v>
       </c>
       <c r="E87" t="n">
-        <v>0.9060290527343751</v>
+        <v>0.9317696228027343</v>
       </c>
     </row>
     <row r="88">
@@ -2099,13 +2099,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>7552.116882324219</v>
+        <v>74993.32000732422</v>
       </c>
       <c r="D88" t="n">
-        <v>-2447.883117675781</v>
+        <v>-25006.67999267578</v>
       </c>
       <c r="E88" t="n">
-        <v>-24.47883117675781</v>
+        <v>-25.00667999267578</v>
       </c>
     </row>
     <row r="89">
@@ -2118,13 +2118,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>9665.878259658813</v>
+        <v>96643.35412979126</v>
       </c>
       <c r="D89" t="n">
-        <v>-334.1217403411865</v>
+        <v>-3356.64587020874</v>
       </c>
       <c r="E89" t="n">
-        <v>-3.341217403411866</v>
+        <v>-3.35664587020874</v>
       </c>
     </row>
     <row r="90">
@@ -2137,13 +2137,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>7034.2780418396</v>
+        <v>70309.81256103516</v>
       </c>
       <c r="D90" t="n">
-        <v>-2965.7219581604</v>
+        <v>-29690.18743896484</v>
       </c>
       <c r="E90" t="n">
-        <v>-29.657219581604</v>
+        <v>-29.69018743896484</v>
       </c>
     </row>
     <row r="91">
@@ -2156,13 +2156,13 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>11696.08029174805</v>
+        <v>117120.6030578613</v>
       </c>
       <c r="D91" t="n">
-        <v>1696.080291748047</v>
+        <v>17120.60305786133</v>
       </c>
       <c r="E91" t="n">
-        <v>16.96080291748047</v>
+        <v>17.12060305786133</v>
       </c>
     </row>
     <row r="92">
@@ -2175,13 +2175,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>9583.551452636719</v>
+        <v>95794.33639526367</v>
       </c>
       <c r="D92" t="n">
-        <v>-416.4485473632812</v>
+        <v>-4205.663604736328</v>
       </c>
       <c r="E92" t="n">
-        <v>-4.164485473632813</v>
+        <v>-4.205663604736328</v>
       </c>
     </row>
     <row r="93">
@@ -2194,13 +2194,13 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>8632.217576980591</v>
+        <v>86306.32374000549</v>
       </c>
       <c r="D93" t="n">
-        <v>-1367.782423019409</v>
+        <v>-13693.67625999451</v>
       </c>
       <c r="E93" t="n">
-        <v>-13.67782423019409</v>
+        <v>-13.69367625999451</v>
       </c>
     </row>
     <row r="94">
@@ -2213,13 +2213,13 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>9013.508411407471</v>
+        <v>90113.59481430054</v>
       </c>
       <c r="D94" t="n">
-        <v>-986.4915885925293</v>
+        <v>-9886.405185699463</v>
       </c>
       <c r="E94" t="n">
-        <v>-9.864915885925294</v>
+        <v>-9.886405185699463</v>
       </c>
     </row>
     <row r="95">
@@ -2232,13 +2232,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7095.848114728928</v>
+        <v>70955.96525549889</v>
       </c>
       <c r="D95" t="n">
-        <v>-2904.151885271072</v>
+        <v>-29044.03474450111</v>
       </c>
       <c r="E95" t="n">
-        <v>-29.04151885271072</v>
+        <v>-29.04403474450111</v>
       </c>
     </row>
     <row r="96">
@@ -2251,13 +2251,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>9273.245998382568</v>
+        <v>92704.73008346558</v>
       </c>
       <c r="D96" t="n">
-        <v>-726.7540016174316</v>
+        <v>-7295.269916534424</v>
       </c>
       <c r="E96" t="n">
-        <v>-7.267540016174316</v>
+        <v>-7.295269916534424</v>
       </c>
     </row>
     <row r="97">
@@ -2270,13 +2270,13 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>11484.32191467285</v>
+        <v>114809.8591842651</v>
       </c>
       <c r="D97" t="n">
-        <v>1484.321914672852</v>
+        <v>14809.85918426514</v>
       </c>
       <c r="E97" t="n">
-        <v>14.84321914672852</v>
+        <v>14.80985918426514</v>
       </c>
     </row>
     <row r="98">
@@ -2289,13 +2289,13 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>15486.30938267708</v>
+        <v>154862.9538267851</v>
       </c>
       <c r="D98" t="n">
-        <v>5486.309382677078</v>
+        <v>54862.95382678509</v>
       </c>
       <c r="E98" t="n">
-        <v>54.86309382677078</v>
+        <v>54.86295382678509</v>
       </c>
     </row>
     <row r="99">
@@ -2308,13 +2308,13 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>10629.00513696671</v>
+        <v>106281.4028739929</v>
       </c>
       <c r="D99" t="n">
-        <v>629.0051369667053</v>
+        <v>6281.40287399292</v>
       </c>
       <c r="E99" t="n">
-        <v>6.290051369667053</v>
+        <v>6.28140287399292</v>
       </c>
     </row>
     <row r="100">
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
@@ -2346,13 +2346,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>10026.87417411804</v>
+        <v>100265.757648468</v>
       </c>
       <c r="D101" t="n">
-        <v>26.87417411804199</v>
+        <v>265.7576484680176</v>
       </c>
       <c r="E101" t="n">
-        <v>0.2687417411804199</v>
+        <v>0.2657576484680176</v>
       </c>
     </row>
     <row r="102">
@@ -2365,13 +2365,13 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11577.80912017822</v>
+        <v>115779.6211872101</v>
       </c>
       <c r="D102" t="n">
-        <v>1577.809120178223</v>
+        <v>15779.62118721008</v>
       </c>
       <c r="E102" t="n">
-        <v>15.77809120178223</v>
+        <v>15.77962118721008</v>
       </c>
     </row>
     <row r="103">
@@ -2384,13 +2384,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>9942.918830871582</v>
+        <v>99421.22149658203</v>
       </c>
       <c r="D103" t="n">
-        <v>-57.08116912841797</v>
+        <v>-578.7785034179688</v>
       </c>
       <c r="E103" t="n">
-        <v>-0.5708116912841797</v>
+        <v>-0.5787785034179688</v>
       </c>
     </row>
     <row r="104">
@@ -2403,13 +2403,13 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>8265.343551635742</v>
+        <v>82619.98218536377</v>
       </c>
       <c r="D104" t="n">
-        <v>-1734.656448364258</v>
+        <v>-17380.01781463623</v>
       </c>
       <c r="E104" t="n">
-        <v>-17.34656448364258</v>
+        <v>-17.38001781463623</v>
       </c>
     </row>
     <row r="105">
@@ -2422,13 +2422,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>9984.240211486816</v>
+        <v>99807.08399200439</v>
       </c>
       <c r="D105" t="n">
-        <v>-15.75978851318359</v>
+        <v>-192.9160079956055</v>
       </c>
       <c r="E105" t="n">
-        <v>-0.1575978851318359</v>
+        <v>-0.1929160079956055</v>
       </c>
     </row>
     <row r="106">
@@ -2441,13 +2441,13 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>14874.70025634766</v>
+        <v>149580.8625183105</v>
       </c>
       <c r="D106" t="n">
-        <v>4874.700256347656</v>
+        <v>49580.86251831055</v>
       </c>
       <c r="E106" t="n">
-        <v>48.74700256347656</v>
+        <v>49.58086251831055</v>
       </c>
     </row>
     <row r="107">
@@ -2460,13 +2460,13 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>12847.29808807373</v>
+        <v>128503.8126564026</v>
       </c>
       <c r="D107" t="n">
-        <v>2847.29808807373</v>
+        <v>28503.81265640259</v>
       </c>
       <c r="E107" t="n">
-        <v>28.4729808807373</v>
+        <v>28.50381265640259</v>
       </c>
     </row>
     <row r="108">
@@ -2479,13 +2479,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>9959.55553817749</v>
+        <v>99573.71068572998</v>
       </c>
       <c r="D108" t="n">
-        <v>-40.44446182250977</v>
+        <v>-426.2893142700195</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.4044446182250976</v>
+        <v>-0.4262893142700196</v>
       </c>
     </row>
     <row r="109">
@@ -2498,13 +2498,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>7135.517200469971</v>
+        <v>71324.9354839325</v>
       </c>
       <c r="D109" t="n">
-        <v>-2864.482799530029</v>
+        <v>-28675.0645160675</v>
       </c>
       <c r="E109" t="n">
-        <v>-28.64482799530029</v>
+        <v>-28.6750645160675</v>
       </c>
     </row>
     <row r="110">
@@ -2517,13 +2517,13 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>8710.250972747803</v>
+        <v>87091.01580905914</v>
       </c>
       <c r="D110" t="n">
-        <v>-1289.749027252197</v>
+        <v>-12908.98419094086</v>
       </c>
       <c r="E110" t="n">
-        <v>-12.89749027252197</v>
+        <v>-12.90898419094086</v>
       </c>
     </row>
     <row r="111">
@@ -2536,13 +2536,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>7532.500356674194</v>
+        <v>75289.50588226318</v>
       </c>
       <c r="D111" t="n">
-        <v>-2467.499643325806</v>
+        <v>-24710.49411773682</v>
       </c>
       <c r="E111" t="n">
-        <v>-24.67499643325806</v>
+        <v>-24.71049411773682</v>
       </c>
     </row>
     <row r="112">
@@ -2555,13 +2555,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>8559.135702133179</v>
+        <v>85591.64650154114</v>
       </c>
       <c r="D112" t="n">
-        <v>-1440.864297866821</v>
+        <v>-14408.35349845886</v>
       </c>
       <c r="E112" t="n">
-        <v>-14.40864297866821</v>
+        <v>-14.40835349845886</v>
       </c>
     </row>
     <row r="113">
@@ -2574,13 +2574,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>7115.648937225342</v>
+        <v>71104.10936737061</v>
       </c>
       <c r="D113" t="n">
-        <v>-2884.351062774658</v>
+        <v>-28895.89063262939</v>
       </c>
       <c r="E113" t="n">
-        <v>-28.84351062774658</v>
+        <v>-28.8958906326294</v>
       </c>
     </row>
     <row r="114">
@@ -2593,13 +2593,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>8701.03568649292</v>
+        <v>87001.94913673401</v>
       </c>
       <c r="D114" t="n">
-        <v>-1298.96431350708</v>
+        <v>-12998.05086326599</v>
       </c>
       <c r="E114" t="n">
-        <v>-12.9896431350708</v>
+        <v>-12.99805086326599</v>
       </c>
     </row>
     <row r="115">
@@ -2612,13 +2612,13 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>6187.849876403809</v>
+        <v>61812.43875694275</v>
       </c>
       <c r="D115" t="n">
-        <v>-3812.150123596191</v>
+        <v>-38187.56124305725</v>
       </c>
       <c r="E115" t="n">
-        <v>-38.12150123596192</v>
+        <v>-38.18756124305725</v>
       </c>
     </row>
     <row r="116">
@@ -2631,13 +2631,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>8853.887338638306</v>
+        <v>88531.3144197464</v>
       </c>
       <c r="D116" t="n">
-        <v>-1146.112661361694</v>
+        <v>-11468.6855802536</v>
       </c>
       <c r="E116" t="n">
-        <v>-11.46112661361694</v>
+        <v>-11.4686855802536</v>
       </c>
     </row>
     <row r="117">
@@ -2650,13 +2650,13 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>12357.74008178711</v>
+        <v>123973.9307556152</v>
       </c>
       <c r="D117" t="n">
-        <v>2357.740081787109</v>
+        <v>23973.93075561523</v>
       </c>
       <c r="E117" t="n">
-        <v>23.57740081787109</v>
+        <v>23.97393075561523</v>
       </c>
     </row>
     <row r="118">
@@ -2669,13 +2669,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>7716.059799194336</v>
+        <v>77098.65796470642</v>
       </c>
       <c r="D118" t="n">
-        <v>-2283.940200805664</v>
+        <v>-22901.34203529358</v>
       </c>
       <c r="E118" t="n">
-        <v>-22.83940200805664</v>
+        <v>-22.90134203529358</v>
       </c>
     </row>
     <row r="119">
@@ -2688,13 +2688,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>8434.812103271484</v>
+        <v>84247.34219741821</v>
       </c>
       <c r="D119" t="n">
-        <v>-1565.187896728516</v>
+        <v>-15752.65780258179</v>
       </c>
       <c r="E119" t="n">
-        <v>-15.65187896728516</v>
+        <v>-15.75265780258179</v>
       </c>
     </row>
     <row r="120">
@@ -2707,13 +2707,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>6269.699258804321</v>
+        <v>62656.01256752014</v>
       </c>
       <c r="D120" t="n">
-        <v>-3730.300741195679</v>
+        <v>-37343.98743247986</v>
       </c>
       <c r="E120" t="n">
-        <v>-37.30300741195678</v>
+        <v>-37.34398743247986</v>
       </c>
     </row>
     <row r="121">
@@ -2726,13 +2726,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>11416.23065567017</v>
+        <v>114163.7169709206</v>
       </c>
       <c r="D121" t="n">
-        <v>1416.230655670166</v>
+        <v>14163.71697092056</v>
       </c>
       <c r="E121" t="n">
-        <v>14.16230655670166</v>
+        <v>14.16371697092056</v>
       </c>
     </row>
     <row r="122">
@@ -2745,13 +2745,13 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>10428.74942779541</v>
+        <v>104348.6342468262</v>
       </c>
       <c r="D122" t="n">
-        <v>428.7494277954102</v>
+        <v>4348.634246826172</v>
       </c>
       <c r="E122" t="n">
-        <v>4.287494277954101</v>
+        <v>4.348634246826172</v>
       </c>
     </row>
     <row r="123">
@@ -2764,13 +2764,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>8602.229789733887</v>
+        <v>85942.73793029785</v>
       </c>
       <c r="D123" t="n">
-        <v>-1397.770210266113</v>
+        <v>-14057.26206970215</v>
       </c>
       <c r="E123" t="n">
-        <v>-13.97770210266113</v>
+        <v>-14.05726206970215</v>
       </c>
     </row>
     <row r="124">
@@ -2783,13 +2783,13 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>11116.78042602539</v>
+        <v>111270.224319458</v>
       </c>
       <c r="D124" t="n">
-        <v>1116.780426025391</v>
+        <v>11270.22431945801</v>
       </c>
       <c r="E124" t="n">
-        <v>11.16780426025391</v>
+        <v>11.27022431945801</v>
       </c>
     </row>
     <row r="125">
@@ -2802,13 +2802,13 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>11379.13427734375</v>
+        <v>114590.0382080078</v>
       </c>
       <c r="D125" t="n">
-        <v>1379.13427734375</v>
+        <v>14590.03820800781</v>
       </c>
       <c r="E125" t="n">
-        <v>13.7913427734375</v>
+        <v>14.59003820800781</v>
       </c>
     </row>
     <row r="126">
@@ -2821,13 +2821,13 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>12117.77757263184</v>
+        <v>121326.219039917</v>
       </c>
       <c r="D126" t="n">
-        <v>2117.777572631836</v>
+        <v>21326.21903991699</v>
       </c>
       <c r="E126" t="n">
-        <v>21.17777572631836</v>
+        <v>21.32621903991699</v>
       </c>
     </row>
     <row r="127">
@@ -2840,13 +2840,13 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>7615.220155715942</v>
+        <v>76151.9315662384</v>
       </c>
       <c r="D127" t="n">
-        <v>-2384.779844284058</v>
+        <v>-23848.0684337616</v>
       </c>
       <c r="E127" t="n">
-        <v>-23.84779844284058</v>
+        <v>-23.8480684337616</v>
       </c>
     </row>
     <row r="128">
@@ -2859,13 +2859,13 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6914.610123634338</v>
+        <v>69128.5512342453</v>
       </c>
       <c r="D128" t="n">
-        <v>-3085.389876365662</v>
+        <v>-30871.4487657547</v>
       </c>
       <c r="E128" t="n">
-        <v>-30.85389876365662</v>
+        <v>-30.8714487657547</v>
       </c>
     </row>
     <row r="129">
@@ -2878,13 +2878,13 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>10111.53840255737</v>
+        <v>101120.9239883423</v>
       </c>
       <c r="D129" t="n">
-        <v>111.538402557373</v>
+        <v>1120.923988342285</v>
       </c>
       <c r="E129" t="n">
-        <v>1.11538402557373</v>
+        <v>1.120923988342285</v>
       </c>
     </row>
     <row r="130">
@@ -2897,13 +2897,13 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>9784.163639068604</v>
+        <v>97842.93194389343</v>
       </c>
       <c r="D130" t="n">
-        <v>-215.8363609313965</v>
+        <v>-2157.068056106567</v>
       </c>
       <c r="E130" t="n">
-        <v>-2.158363609313965</v>
+        <v>-2.157068056106568</v>
       </c>
     </row>
     <row r="131">
@@ -2916,13 +2916,13 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>10811.22975158691</v>
+        <v>108201.1974716187</v>
       </c>
       <c r="D131" t="n">
-        <v>811.2297515869141</v>
+        <v>8201.197471618652</v>
       </c>
       <c r="E131" t="n">
-        <v>8.112297515869141</v>
+        <v>8.201197471618652</v>
       </c>
     </row>
     <row r="132">
@@ -2935,13 +2935,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>6770.730340957642</v>
+        <v>67688.45340919495</v>
       </c>
       <c r="D132" t="n">
-        <v>-3229.269659042358</v>
+        <v>-32311.54659080505</v>
       </c>
       <c r="E132" t="n">
-        <v>-32.29269659042359</v>
+        <v>-32.31154659080505</v>
       </c>
     </row>
     <row r="133">
@@ -2954,13 +2954,13 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>6111.921028137207</v>
+        <v>61098.62028884888</v>
       </c>
       <c r="D133" t="n">
-        <v>-3888.078971862793</v>
+        <v>-38901.37971115112</v>
       </c>
       <c r="E133" t="n">
-        <v>-38.88078971862793</v>
+        <v>-38.90137971115112</v>
       </c>
     </row>
     <row r="134">
@@ -2973,13 +2973,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>23156.3943157196</v>
+        <v>231896.5905952454</v>
       </c>
       <c r="D134" t="n">
-        <v>13156.3943157196</v>
+        <v>131896.5905952454</v>
       </c>
       <c r="E134" t="n">
-        <v>131.563943157196</v>
+        <v>131.8965905952454</v>
       </c>
     </row>
     <row r="135">
@@ -2992,13 +2992,13 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>10052.56942033768</v>
+        <v>100525.0842018127</v>
       </c>
       <c r="D135" t="n">
-        <v>52.569420337677</v>
+        <v>525.0842018127441</v>
       </c>
       <c r="E135" t="n">
-        <v>0.52569420337677</v>
+        <v>0.5250842018127442</v>
       </c>
     </row>
     <row r="136">
@@ -3011,13 +3011,13 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>11291.03067159653</v>
+        <v>112915.426718235</v>
       </c>
       <c r="D136" t="n">
-        <v>1291.030671596527</v>
+        <v>12915.42671823502</v>
       </c>
       <c r="E136" t="n">
-        <v>12.91030671596527</v>
+        <v>12.91542671823501</v>
       </c>
     </row>
     <row r="137">
@@ -3030,13 +3030,13 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>9983.04043006897</v>
+        <v>99834.12429904938</v>
       </c>
       <c r="D137" t="n">
-        <v>-16.95956993103027</v>
+        <v>-165.8757009506226</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.1695956993103027</v>
+        <v>-0.1658757009506225</v>
       </c>
     </row>
     <row r="138">
@@ -3049,13 +3049,13 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>9840.000244140625</v>
+        <v>98376.63759422302</v>
       </c>
       <c r="D138" t="n">
-        <v>-159.999755859375</v>
+        <v>-1623.362405776978</v>
       </c>
       <c r="E138" t="n">
-        <v>-1.59999755859375</v>
+        <v>-1.623362405776977</v>
       </c>
     </row>
     <row r="139">
@@ -3068,13 +3068,13 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>9968.624618530273</v>
+        <v>99655.79009246826</v>
       </c>
       <c r="D139" t="n">
-        <v>-31.37538146972656</v>
+        <v>-344.2099075317383</v>
       </c>
       <c r="E139" t="n">
-        <v>-0.3137538146972657</v>
+        <v>-0.3442099075317382</v>
       </c>
     </row>
     <row r="140">
@@ -3087,13 +3087,13 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>10638.6973400116</v>
+        <v>106387.635723114</v>
       </c>
       <c r="D140" t="n">
-        <v>638.6973400115967</v>
+        <v>6387.635723114014</v>
       </c>
       <c r="E140" t="n">
-        <v>6.386973400115966</v>
+        <v>6.387635723114014</v>
       </c>
     </row>
     <row r="141">
@@ -3106,13 +3106,13 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>12116.46789550781</v>
+        <v>121379.5859375</v>
       </c>
       <c r="D141" t="n">
-        <v>2116.467895507812</v>
+        <v>21379.5859375</v>
       </c>
       <c r="E141" t="n">
-        <v>21.16467895507813</v>
+        <v>21.3795859375</v>
       </c>
     </row>
     <row r="142">
@@ -3125,13 +3125,13 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>10699.57135772705</v>
+        <v>107016.5700302124</v>
       </c>
       <c r="D142" t="n">
-        <v>699.5713577270508</v>
+        <v>7016.570030212402</v>
       </c>
       <c r="E142" t="n">
-        <v>6.995713577270508</v>
+        <v>7.016570030212402</v>
       </c>
     </row>
     <row r="143">
@@ -3144,13 +3144,13 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>12193.37301921844</v>
+        <v>122012.5880861282</v>
       </c>
       <c r="D143" t="n">
-        <v>2193.373019218445</v>
+        <v>22012.58808612823</v>
       </c>
       <c r="E143" t="n">
-        <v>21.93373019218445</v>
+        <v>22.01258808612824</v>
       </c>
     </row>
     <row r="144">
@@ -3163,13 +3163,13 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>8992.909034729004</v>
+        <v>89891.6614112854</v>
       </c>
       <c r="D144" t="n">
-        <v>-1007.090965270996</v>
+        <v>-10108.3385887146</v>
       </c>
       <c r="E144" t="n">
-        <v>-10.07090965270996</v>
+        <v>-10.1083385887146</v>
       </c>
     </row>
     <row r="145">
@@ -3182,13 +3182,13 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>12394.12112426758</v>
+        <v>123955.0502548218</v>
       </c>
       <c r="D145" t="n">
-        <v>2394.121124267578</v>
+        <v>23955.05025482178</v>
       </c>
       <c r="E145" t="n">
-        <v>23.94121124267578</v>
+        <v>23.95505025482178</v>
       </c>
     </row>
     <row r="146">
@@ -3201,13 +3201,13 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>16078.83531665802</v>
+        <v>160804.5859537125</v>
       </c>
       <c r="D146" t="n">
-        <v>6078.83531665802</v>
+        <v>60804.58595371246</v>
       </c>
       <c r="E146" t="n">
-        <v>60.7883531665802</v>
+        <v>60.80458595371246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   decimalodd.ipynb 	modified:   decimalodd_res/bb.xlsx 	modified:   decimalodd_res/macd.xlsx 	modified:   decimalodd_res/obv.xlsx 	modified:   winrate_result/bb.xlsx 	modified:   winrate_result/macd.xlsx 	modified:   winrate_result/obv.xlsx 	modified:   winrate_test.ipynb
</commit_message>
<xml_diff>
--- a/decimalodd_res/macd.xlsx
+++ b/decimalodd_res/macd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>119694.7937469482</v>
+        <v>119694.7878189087</v>
       </c>
       <c r="D2" t="n">
-        <v>19694.79374694824</v>
+        <v>19694.78781890869</v>
       </c>
       <c r="E2" t="n">
-        <v>19.69479374694824</v>
+        <v>19.69478781890869</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>123477.6673431396</v>
+        <v>123477.6890716553</v>
       </c>
       <c r="D3" t="n">
-        <v>23477.66734313965</v>
+        <v>23477.68907165527</v>
       </c>
       <c r="E3" t="n">
-        <v>23.47766734313965</v>
+        <v>23.47768907165527</v>
       </c>
     </row>
     <row r="4">
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>110926.5220222473</v>
+        <v>110926.4676971436</v>
       </c>
       <c r="D4" t="n">
-        <v>10926.52202224731</v>
+        <v>10926.46769714355</v>
       </c>
       <c r="E4" t="n">
-        <v>10.92652202224732</v>
+        <v>10.92646769714355</v>
       </c>
     </row>
     <row r="5">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>111900.5071563721</v>
+        <v>111900.4582061768</v>
       </c>
       <c r="D6" t="n">
-        <v>11900.50715637207</v>
+        <v>11900.45820617676</v>
       </c>
       <c r="E6" t="n">
-        <v>11.90050715637207</v>
+        <v>11.90045820617676</v>
       </c>
     </row>
     <row r="7">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>106710.4298629761</v>
+        <v>106710.5300750732</v>
       </c>
       <c r="D8" t="n">
-        <v>6710.429862976074</v>
+        <v>6710.530075073242</v>
       </c>
       <c r="E8" t="n">
-        <v>6.710429862976073</v>
+        <v>6.710530075073243</v>
       </c>
     </row>
     <row r="9">
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>112959.9247589111</v>
+        <v>112959.9361114502</v>
       </c>
       <c r="D9" t="n">
-        <v>12959.92475891113</v>
+        <v>12959.9361114502</v>
       </c>
       <c r="E9" t="n">
-        <v>12.95992475891113</v>
+        <v>12.9599361114502</v>
       </c>
     </row>
     <row r="10">
@@ -617,13 +617,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>123259.4151859283</v>
+        <v>123259.421579361</v>
       </c>
       <c r="D10" t="n">
-        <v>23259.41518592834</v>
+        <v>23259.42157936096</v>
       </c>
       <c r="E10" t="n">
-        <v>23.25941518592834</v>
+        <v>23.25942157936096</v>
       </c>
     </row>
     <row r="11">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>101058.291595459</v>
+        <v>101058.3901824951</v>
       </c>
       <c r="D11" t="n">
-        <v>1058.291595458984</v>
+        <v>1058.390182495117</v>
       </c>
       <c r="E11" t="n">
-        <v>1.058291595458984</v>
+        <v>1.058390182495117</v>
       </c>
     </row>
     <row r="12">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>100437.4589424133</v>
+        <v>100438.547492981</v>
       </c>
       <c r="D12" t="n">
-        <v>437.4589424133301</v>
+        <v>438.547492980957</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4374589424133301</v>
+        <v>0.438547492980957</v>
       </c>
     </row>
     <row r="13">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>108449.3448524475</v>
+        <v>108449.3148841858</v>
       </c>
       <c r="D13" t="n">
-        <v>8449.34485244751</v>
+        <v>8449.314884185791</v>
       </c>
       <c r="E13" t="n">
-        <v>8.44934485244751</v>
+        <v>8.449314884185791</v>
       </c>
     </row>
     <row r="14">
@@ -693,13 +693,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>114942.1506690979</v>
+        <v>114942.1409263611</v>
       </c>
       <c r="D14" t="n">
-        <v>14942.1506690979</v>
+        <v>14942.14092636108</v>
       </c>
       <c r="E14" t="n">
-        <v>14.9421506690979</v>
+        <v>14.94214092636108</v>
       </c>
     </row>
     <row r="15">
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>113758.5279846191</v>
+        <v>113758.5175933838</v>
       </c>
       <c r="D15" t="n">
-        <v>13758.52798461914</v>
+        <v>13758.51759338379</v>
       </c>
       <c r="E15" t="n">
-        <v>13.75852798461914</v>
+        <v>13.75851759338379</v>
       </c>
     </row>
     <row r="16">
@@ -731,13 +731,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>88971.87142181396</v>
+        <v>88971.9017868042</v>
       </c>
       <c r="D16" t="n">
-        <v>-11028.12857818604</v>
+        <v>-11028.0982131958</v>
       </c>
       <c r="E16" t="n">
-        <v>-11.02812857818603</v>
+        <v>-11.0280982131958</v>
       </c>
     </row>
     <row r="17">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>120207.0395202637</v>
+        <v>120206.9701271057</v>
       </c>
       <c r="D17" t="n">
-        <v>20207.03952026367</v>
+        <v>20206.97012710571</v>
       </c>
       <c r="E17" t="n">
-        <v>20.20703952026367</v>
+        <v>20.20697012710571</v>
       </c>
     </row>
     <row r="18">
@@ -769,13 +769,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>126553.3456268311</v>
+        <v>126542.7050323486</v>
       </c>
       <c r="D18" t="n">
-        <v>26553.34562683105</v>
+        <v>26542.70503234863</v>
       </c>
       <c r="E18" t="n">
-        <v>26.55334562683105</v>
+        <v>26.54270503234864</v>
       </c>
     </row>
     <row r="19">
@@ -788,13 +788,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>123715.6070022583</v>
+        <v>124467.1721687317</v>
       </c>
       <c r="D19" t="n">
-        <v>23715.6070022583</v>
+        <v>24467.17216873169</v>
       </c>
       <c r="E19" t="n">
-        <v>23.7156070022583</v>
+        <v>24.46717216873169</v>
       </c>
     </row>
     <row r="20">
@@ -807,13 +807,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>83014.82019805908</v>
+        <v>83014.8770866394</v>
       </c>
       <c r="D20" t="n">
-        <v>-16985.17980194092</v>
+        <v>-16985.1229133606</v>
       </c>
       <c r="E20" t="n">
-        <v>-16.98517980194092</v>
+        <v>-16.98512291336059</v>
       </c>
     </row>
     <row r="21">
@@ -826,13 +826,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>91663.25539779663</v>
+        <v>91663.2774810791</v>
       </c>
       <c r="D21" t="n">
-        <v>-8336.744602203369</v>
+        <v>-8336.722518920898</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.336744602203369</v>
+        <v>-8.336722518920899</v>
       </c>
     </row>
     <row r="22">
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>128907.0210113525</v>
+        <v>128907.1228485107</v>
       </c>
       <c r="D22" t="n">
-        <v>28907.02101135254</v>
+        <v>28907.12284851074</v>
       </c>
       <c r="E22" t="n">
-        <v>28.90702101135254</v>
+        <v>28.90712284851074</v>
       </c>
     </row>
     <row r="23">
@@ -864,13 +864,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>104806.0463562012</v>
+        <v>104806.0942840576</v>
       </c>
       <c r="D23" t="n">
-        <v>4806.046356201172</v>
+        <v>4806.094284057617</v>
       </c>
       <c r="E23" t="n">
-        <v>4.806046356201172</v>
+        <v>4.806094284057617</v>
       </c>
     </row>
     <row r="24">
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>92416.45233535767</v>
+        <v>92416.47953796387</v>
       </c>
       <c r="D24" t="n">
-        <v>-7583.547664642334</v>
+        <v>-7583.520462036133</v>
       </c>
       <c r="E24" t="n">
-        <v>-7.583547664642334</v>
+        <v>-7.583520462036134</v>
       </c>
     </row>
     <row r="25">
@@ -902,13 +902,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>127995.5507202148</v>
+        <v>127995.54347229</v>
       </c>
       <c r="D25" t="n">
-        <v>27995.55072021484</v>
+        <v>27995.54347229004</v>
       </c>
       <c r="E25" t="n">
-        <v>27.99555072021484</v>
+        <v>27.99554347229004</v>
       </c>
     </row>
     <row r="26">
@@ -921,13 +921,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>114213.0182418823</v>
+        <v>114212.992767334</v>
       </c>
       <c r="D26" t="n">
-        <v>14213.01824188232</v>
+        <v>14212.99276733398</v>
       </c>
       <c r="E26" t="n">
-        <v>14.21301824188232</v>
+        <v>14.21299276733398</v>
       </c>
     </row>
     <row r="27">
@@ -940,13 +940,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>115368.2472991943</v>
+        <v>115368.3167419434</v>
       </c>
       <c r="D27" t="n">
-        <v>15368.24729919434</v>
+        <v>15368.31674194336</v>
       </c>
       <c r="E27" t="n">
-        <v>15.36824729919434</v>
+        <v>15.36831674194336</v>
       </c>
     </row>
     <row r="28">
@@ -959,13 +959,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>114075.2806625366</v>
+        <v>114075.1840820312</v>
       </c>
       <c r="D28" t="n">
-        <v>14075.28066253662</v>
+        <v>14075.18408203125</v>
       </c>
       <c r="E28" t="n">
-        <v>14.07528066253662</v>
+        <v>14.07518408203125</v>
       </c>
     </row>
     <row r="29">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>136048.807800293</v>
+        <v>136048.8297424316</v>
       </c>
       <c r="D29" t="n">
-        <v>36048.80780029297</v>
+        <v>36048.82974243164</v>
       </c>
       <c r="E29" t="n">
-        <v>36.04880780029297</v>
+        <v>36.04882974243164</v>
       </c>
     </row>
     <row r="30">
@@ -1016,13 +1016,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>101103.3532676697</v>
+        <v>101103.3436012268</v>
       </c>
       <c r="D31" t="n">
-        <v>1103.353267669678</v>
+        <v>1103.343601226807</v>
       </c>
       <c r="E31" t="n">
-        <v>1.103353267669678</v>
+        <v>1.103343601226807</v>
       </c>
     </row>
     <row r="32">
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>102812.4024772644</v>
+        <v>102812.4752502441</v>
       </c>
       <c r="D33" t="n">
-        <v>2812.402477264404</v>
+        <v>2812.475250244141</v>
       </c>
       <c r="E33" t="n">
-        <v>2.812402477264405</v>
+        <v>2.812475250244141</v>
       </c>
     </row>
     <row r="34">
@@ -1073,13 +1073,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>79094.5196685791</v>
+        <v>79094.48710632324</v>
       </c>
       <c r="D34" t="n">
-        <v>-20905.4803314209</v>
+        <v>-20905.51289367676</v>
       </c>
       <c r="E34" t="n">
-        <v>-20.9054803314209</v>
+        <v>-20.90551289367676</v>
       </c>
     </row>
     <row r="35">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>141016.3170471191</v>
+        <v>141016.3223495483</v>
       </c>
       <c r="D35" t="n">
-        <v>41016.31704711914</v>
+        <v>41016.32234954834</v>
       </c>
       <c r="E35" t="n">
-        <v>41.01631704711914</v>
+        <v>41.01632234954834</v>
       </c>
     </row>
     <row r="36">
@@ -1111,13 +1111,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>104317.9474334717</v>
+        <v>104317.9369888306</v>
       </c>
       <c r="D36" t="n">
-        <v>4317.94743347168</v>
+        <v>4317.936988830566</v>
       </c>
       <c r="E36" t="n">
-        <v>4.31794743347168</v>
+        <v>4.317936988830566</v>
       </c>
     </row>
     <row r="37">
@@ -1130,13 +1130,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>96889.24454116821</v>
+        <v>96892.67601013184</v>
       </c>
       <c r="D37" t="n">
-        <v>-3110.755458831787</v>
+        <v>-3107.323989868164</v>
       </c>
       <c r="E37" t="n">
-        <v>-3.110755458831787</v>
+        <v>-3.107323989868164</v>
       </c>
     </row>
     <row r="38">
@@ -1149,13 +1149,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>148272.2018432617</v>
+        <v>148272.237701416</v>
       </c>
       <c r="D38" t="n">
-        <v>48272.20184326172</v>
+        <v>48272.23770141602</v>
       </c>
       <c r="E38" t="n">
-        <v>48.27220184326172</v>
+        <v>48.27223770141602</v>
       </c>
     </row>
     <row r="39">
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>122907.5224914551</v>
+        <v>122907.4830322266</v>
       </c>
       <c r="D39" t="n">
-        <v>22907.52249145508</v>
+        <v>22907.48303222656</v>
       </c>
       <c r="E39" t="n">
-        <v>22.90752249145508</v>
+        <v>22.90748303222657</v>
       </c>
     </row>
     <row r="40">
@@ -1187,13 +1187,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>129383.3076782227</v>
+        <v>129383.2922210693</v>
       </c>
       <c r="D40" t="n">
-        <v>29383.30767822266</v>
+        <v>29383.29222106934</v>
       </c>
       <c r="E40" t="n">
-        <v>29.38330767822266</v>
+        <v>29.38329222106934</v>
       </c>
     </row>
     <row r="41">
@@ -1206,13 +1206,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>105716.2997741699</v>
+        <v>105716.3523330688</v>
       </c>
       <c r="D41" t="n">
-        <v>5716.299774169922</v>
+        <v>5716.352333068848</v>
       </c>
       <c r="E41" t="n">
-        <v>5.716299774169921</v>
+        <v>5.716352333068848</v>
       </c>
     </row>
     <row r="42">
@@ -1244,13 +1244,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>90677.67463684082</v>
+        <v>90677.69345092773</v>
       </c>
       <c r="D43" t="n">
-        <v>-9322.32536315918</v>
+        <v>-9322.306549072266</v>
       </c>
       <c r="E43" t="n">
-        <v>-9.32232536315918</v>
+        <v>-9.322306549072264</v>
       </c>
     </row>
     <row r="44">
@@ -1263,13 +1263,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>121422.9367828369</v>
+        <v>121422.96144104</v>
       </c>
       <c r="D44" t="n">
-        <v>21422.93678283691</v>
+        <v>21422.96144104004</v>
       </c>
       <c r="E44" t="n">
-        <v>21.42293678283691</v>
+        <v>21.42296144104004</v>
       </c>
     </row>
     <row r="45">
@@ -1282,13 +1282,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>104875.0488052368</v>
+        <v>104874.9716262817</v>
       </c>
       <c r="D45" t="n">
-        <v>4875.048805236816</v>
+        <v>4874.971626281738</v>
       </c>
       <c r="E45" t="n">
-        <v>4.875048805236816</v>
+        <v>4.874971626281739</v>
       </c>
     </row>
     <row r="46">
@@ -1301,13 +1301,13 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>114420.8460464478</v>
+        <v>114425.4955787659</v>
       </c>
       <c r="D46" t="n">
-        <v>14420.84604644775</v>
+        <v>14425.49557876587</v>
       </c>
       <c r="E46" t="n">
-        <v>14.42084604644776</v>
+        <v>14.42549557876587</v>
       </c>
     </row>
     <row r="47">
@@ -1320,13 +1320,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>103032.5048675537</v>
+        <v>103032.4696807861</v>
       </c>
       <c r="D47" t="n">
-        <v>3032.504867553711</v>
+        <v>3032.469680786133</v>
       </c>
       <c r="E47" t="n">
-        <v>3.032504867553711</v>
+        <v>3.032469680786133</v>
       </c>
     </row>
     <row r="48">
@@ -1339,13 +1339,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>121722.1455535889</v>
+        <v>121722.1026000977</v>
       </c>
       <c r="D48" t="n">
-        <v>21722.14555358887</v>
+        <v>21722.10260009766</v>
       </c>
       <c r="E48" t="n">
-        <v>21.72214555358887</v>
+        <v>21.72210260009766</v>
       </c>
     </row>
     <row r="49">
@@ -1358,13 +1358,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>108312.7405395508</v>
+        <v>108312.806678772</v>
       </c>
       <c r="D49" t="n">
-        <v>8312.740539550781</v>
+        <v>8312.806678771973</v>
       </c>
       <c r="E49" t="n">
-        <v>8.312740539550781</v>
+        <v>8.312806678771972</v>
       </c>
     </row>
     <row r="50">
@@ -1396,13 +1396,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>109380.7565765381</v>
+        <v>109380.7922210693</v>
       </c>
       <c r="D51" t="n">
-        <v>9380.756576538086</v>
+        <v>9380.792221069336</v>
       </c>
       <c r="E51" t="n">
-        <v>9.380756576538086</v>
+        <v>9.380792221069335</v>
       </c>
     </row>
     <row r="52">
@@ -1434,13 +1434,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>103474.6545181274</v>
+        <v>103474.574546814</v>
       </c>
       <c r="D53" t="n">
-        <v>3474.654518127441</v>
+        <v>3474.574546813965</v>
       </c>
       <c r="E53" t="n">
-        <v>3.474654518127442</v>
+        <v>3.474574546813965</v>
       </c>
     </row>
     <row r="54">
@@ -1453,13 +1453,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>102127.6962070465</v>
+        <v>102126.0927772522</v>
       </c>
       <c r="D54" t="n">
-        <v>2127.696207046509</v>
+        <v>2126.092777252197</v>
       </c>
       <c r="E54" t="n">
-        <v>2.127696207046509</v>
+        <v>2.126092777252197</v>
       </c>
     </row>
     <row r="55">
@@ -1510,13 +1510,13 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>95165.48588562012</v>
+        <v>95165.41743469238</v>
       </c>
       <c r="D57" t="n">
-        <v>-4834.514114379883</v>
+        <v>-4834.582565307617</v>
       </c>
       <c r="E57" t="n">
-        <v>-4.834514114379883</v>
+        <v>-4.834582565307617</v>
       </c>
     </row>
     <row r="58">
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>116036.8251304626</v>
+        <v>116036.8679542542</v>
       </c>
       <c r="D58" t="n">
-        <v>16036.82513046265</v>
+        <v>16036.86795425415</v>
       </c>
       <c r="E58" t="n">
-        <v>16.03682513046265</v>
+        <v>16.03686795425415</v>
       </c>
     </row>
     <row r="59">
@@ -1567,13 +1567,13 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>84781.00667190552</v>
+        <v>84781.0122718811</v>
       </c>
       <c r="D60" t="n">
-        <v>-15218.99332809448</v>
+        <v>-15218.9877281189</v>
       </c>
       <c r="E60" t="n">
-        <v>-15.21899332809448</v>
+        <v>-15.2189877281189</v>
       </c>
     </row>
     <row r="61">
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>77545.27185821533</v>
+        <v>77545.26863098145</v>
       </c>
       <c r="D61" t="n">
-        <v>-22454.72814178467</v>
+        <v>-22454.73136901855</v>
       </c>
       <c r="E61" t="n">
-        <v>-22.45472814178467</v>
+        <v>-22.45473136901855</v>
       </c>
     </row>
     <row r="62">
@@ -1643,13 +1643,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>118691.3671531677</v>
+        <v>118691.3329658508</v>
       </c>
       <c r="D64" t="n">
-        <v>18691.36715316772</v>
+        <v>18691.33296585083</v>
       </c>
       <c r="E64" t="n">
-        <v>18.69136715316772</v>
+        <v>18.69133296585083</v>
       </c>
     </row>
     <row r="65">
@@ -1681,13 +1681,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>83036.58343315125</v>
+        <v>83036.60769844055</v>
       </c>
       <c r="D66" t="n">
-        <v>-16963.41656684875</v>
+        <v>-16963.39230155945</v>
       </c>
       <c r="E66" t="n">
-        <v>-16.96341656684875</v>
+        <v>-16.96339230155945</v>
       </c>
     </row>
     <row r="67">
@@ -1700,13 +1700,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>124418.7358617783</v>
+        <v>124418.7090265751</v>
       </c>
       <c r="D67" t="n">
-        <v>24418.73586177826</v>
+        <v>24418.70902657509</v>
       </c>
       <c r="E67" t="n">
-        <v>24.41873586177826</v>
+        <v>24.41870902657509</v>
       </c>
     </row>
     <row r="68">
@@ -1757,13 +1757,13 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>116904.8969268799</v>
+        <v>116904.8994140625</v>
       </c>
       <c r="D70" t="n">
-        <v>16904.89692687988</v>
+        <v>16904.8994140625</v>
       </c>
       <c r="E70" t="n">
-        <v>16.90489692687988</v>
+        <v>16.9048994140625</v>
       </c>
     </row>
     <row r="71">
@@ -1833,13 +1833,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>76615.62582588196</v>
+        <v>76615.59383487701</v>
       </c>
       <c r="D74" t="n">
-        <v>-23384.37417411804</v>
+        <v>-23384.40616512299</v>
       </c>
       <c r="E74" t="n">
-        <v>-23.38437417411804</v>
+        <v>-23.38440616512299</v>
       </c>
     </row>
     <row r="75">
@@ -1890,13 +1890,13 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>133297.4388122559</v>
+        <v>133297.4587097168</v>
       </c>
       <c r="D77" t="n">
-        <v>33297.43881225586</v>
+        <v>33297.4587097168</v>
       </c>
       <c r="E77" t="n">
-        <v>33.29743881225586</v>
+        <v>33.2974587097168</v>
       </c>
     </row>
     <row r="78">
@@ -2023,13 +2023,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>121493.9067192078</v>
+        <v>121493.8392944336</v>
       </c>
       <c r="D84" t="n">
-        <v>21493.90671920776</v>
+        <v>21493.83929443359</v>
       </c>
       <c r="E84" t="n">
-        <v>21.49390671920776</v>
+        <v>21.4938392944336</v>
       </c>
     </row>
     <row r="85">
@@ -2042,13 +2042,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>93867.10158157349</v>
+        <v>93867.14140701294</v>
       </c>
       <c r="D85" t="n">
-        <v>-6132.898418426514</v>
+        <v>-6132.858592987061</v>
       </c>
       <c r="E85" t="n">
-        <v>-6.132898418426514</v>
+        <v>-6.13285859298706</v>
       </c>
     </row>
     <row r="86">
@@ -2080,13 +2080,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>100931.7696228027</v>
+        <v>100931.9448394775</v>
       </c>
       <c r="D87" t="n">
-        <v>931.7696228027344</v>
+        <v>931.9448394775391</v>
       </c>
       <c r="E87" t="n">
-        <v>0.9317696228027343</v>
+        <v>0.931944839477539</v>
       </c>
     </row>
     <row r="88">
@@ -2099,13 +2099,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>74993.32000732422</v>
+        <v>74993.34838867188</v>
       </c>
       <c r="D88" t="n">
-        <v>-25006.67999267578</v>
+        <v>-25006.65161132812</v>
       </c>
       <c r="E88" t="n">
-        <v>-25.00667999267578</v>
+        <v>-25.00665161132812</v>
       </c>
     </row>
     <row r="89">
@@ -2118,13 +2118,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>96643.35412979126</v>
+        <v>96643.41440391541</v>
       </c>
       <c r="D89" t="n">
-        <v>-3356.64587020874</v>
+        <v>-3356.585596084595</v>
       </c>
       <c r="E89" t="n">
-        <v>-3.35664587020874</v>
+        <v>-3.356585596084595</v>
       </c>
     </row>
     <row r="90">
@@ -2137,13 +2137,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>70309.81256103516</v>
+        <v>70309.81430435181</v>
       </c>
       <c r="D90" t="n">
-        <v>-29690.18743896484</v>
+        <v>-29690.18569564819</v>
       </c>
       <c r="E90" t="n">
-        <v>-29.69018743896484</v>
+        <v>-29.69018569564819</v>
       </c>
     </row>
     <row r="91">
@@ -2175,13 +2175,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>95794.33639526367</v>
+        <v>95794.38595581055</v>
       </c>
       <c r="D92" t="n">
-        <v>-4205.663604736328</v>
+        <v>-4205.614044189453</v>
       </c>
       <c r="E92" t="n">
-        <v>-4.205663604736328</v>
+        <v>-4.205614044189454</v>
       </c>
     </row>
     <row r="93">
@@ -2194,13 +2194,13 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>86306.32374000549</v>
+        <v>86306.38268661499</v>
       </c>
       <c r="D93" t="n">
-        <v>-13693.67625999451</v>
+        <v>-13693.61731338501</v>
       </c>
       <c r="E93" t="n">
-        <v>-13.69367625999451</v>
+        <v>-13.69361731338501</v>
       </c>
     </row>
     <row r="94">
@@ -2213,13 +2213,13 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>90113.59481430054</v>
+        <v>90113.59375</v>
       </c>
       <c r="D94" t="n">
-        <v>-9886.405185699463</v>
+        <v>-9886.40625</v>
       </c>
       <c r="E94" t="n">
-        <v>-9.886405185699463</v>
+        <v>-9.88640625</v>
       </c>
     </row>
     <row r="95">
@@ -2232,13 +2232,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>70955.96525549889</v>
+        <v>70955.95919704437</v>
       </c>
       <c r="D95" t="n">
-        <v>-29044.03474450111</v>
+        <v>-29044.04080295563</v>
       </c>
       <c r="E95" t="n">
-        <v>-29.04403474450111</v>
+        <v>-29.04404080295563</v>
       </c>
     </row>
     <row r="96">
@@ -2251,13 +2251,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>92704.73008346558</v>
+        <v>92704.73517227173</v>
       </c>
       <c r="D96" t="n">
-        <v>-7295.269916534424</v>
+        <v>-7295.264827728271</v>
       </c>
       <c r="E96" t="n">
-        <v>-7.295269916534424</v>
+        <v>-7.295264827728272</v>
       </c>
     </row>
     <row r="97">
@@ -2308,13 +2308,13 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>106281.4028739929</v>
+        <v>106281.3811030388</v>
       </c>
       <c r="D99" t="n">
-        <v>6281.40287399292</v>
+        <v>6281.381103038788</v>
       </c>
       <c r="E99" t="n">
-        <v>6.28140287399292</v>
+        <v>6.281381103038789</v>
       </c>
     </row>
     <row r="100">
@@ -2346,13 +2346,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>100265.757648468</v>
+        <v>100265.7262306213</v>
       </c>
       <c r="D101" t="n">
-        <v>265.7576484680176</v>
+        <v>265.7262306213379</v>
       </c>
       <c r="E101" t="n">
-        <v>0.2657576484680176</v>
+        <v>0.2657262306213379</v>
       </c>
     </row>
     <row r="102">
@@ -2384,13 +2384,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>99421.22149658203</v>
+        <v>99421.15892028809</v>
       </c>
       <c r="D103" t="n">
-        <v>-578.7785034179688</v>
+        <v>-578.8410797119141</v>
       </c>
       <c r="E103" t="n">
-        <v>-0.5787785034179688</v>
+        <v>-0.578841079711914</v>
       </c>
     </row>
     <row r="104">
@@ -2403,13 +2403,13 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>82619.98218536377</v>
+        <v>82619.93482971191</v>
       </c>
       <c r="D104" t="n">
-        <v>-17380.01781463623</v>
+        <v>-17380.06517028809</v>
       </c>
       <c r="E104" t="n">
-        <v>-17.38001781463623</v>
+        <v>-17.38006517028809</v>
       </c>
     </row>
     <row r="105">
@@ -2422,13 +2422,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>99807.08399200439</v>
+        <v>99806.44418334961</v>
       </c>
       <c r="D105" t="n">
-        <v>-192.9160079956055</v>
+        <v>-193.5558166503906</v>
       </c>
       <c r="E105" t="n">
-        <v>-0.1929160079956055</v>
+        <v>-0.1935558166503906</v>
       </c>
     </row>
     <row r="106">
@@ -2460,13 +2460,13 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>128503.8126564026</v>
+        <v>128503.8633823395</v>
       </c>
       <c r="D107" t="n">
-        <v>28503.81265640259</v>
+        <v>28503.86338233948</v>
       </c>
       <c r="E107" t="n">
-        <v>28.50381265640259</v>
+        <v>28.50386338233948</v>
       </c>
     </row>
     <row r="108">
@@ -2479,13 +2479,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>99573.71068572998</v>
+        <v>99573.71076965332</v>
       </c>
       <c r="D108" t="n">
-        <v>-426.2893142700195</v>
+        <v>-426.2892303466797</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.4262893142700196</v>
+        <v>-0.4262892303466796</v>
       </c>
     </row>
     <row r="109">
@@ -2498,13 +2498,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>71324.9354839325</v>
+        <v>71324.92639350891</v>
       </c>
       <c r="D109" t="n">
-        <v>-28675.0645160675</v>
+        <v>-28675.07360649109</v>
       </c>
       <c r="E109" t="n">
-        <v>-28.6750645160675</v>
+        <v>-28.67507360649109</v>
       </c>
     </row>
     <row r="110">
@@ -2517,13 +2517,13 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>87091.01580905914</v>
+        <v>87090.97622394562</v>
       </c>
       <c r="D110" t="n">
-        <v>-12908.98419094086</v>
+        <v>-12909.02377605438</v>
       </c>
       <c r="E110" t="n">
-        <v>-12.90898419094086</v>
+        <v>-12.90902377605438</v>
       </c>
     </row>
     <row r="111">
@@ -2536,13 +2536,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>75289.50588226318</v>
+        <v>75289.50107765198</v>
       </c>
       <c r="D111" t="n">
-        <v>-24710.49411773682</v>
+        <v>-24710.49892234802</v>
       </c>
       <c r="E111" t="n">
-        <v>-24.71049411773682</v>
+        <v>-24.71049892234802</v>
       </c>
     </row>
     <row r="112">
@@ -2555,13 +2555,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>85591.64650154114</v>
+        <v>85591.66578483582</v>
       </c>
       <c r="D112" t="n">
-        <v>-14408.35349845886</v>
+        <v>-14408.33421516418</v>
       </c>
       <c r="E112" t="n">
-        <v>-14.40835349845886</v>
+        <v>-14.40833421516418</v>
       </c>
     </row>
     <row r="113">
@@ -2574,13 +2574,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>71104.10936737061</v>
+        <v>71104.1342086792</v>
       </c>
       <c r="D113" t="n">
-        <v>-28895.89063262939</v>
+        <v>-28895.8657913208</v>
       </c>
       <c r="E113" t="n">
-        <v>-28.8958906326294</v>
+        <v>-28.8958657913208</v>
       </c>
     </row>
     <row r="114">
@@ -2593,13 +2593,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>87001.94913673401</v>
+        <v>87001.95952796936</v>
       </c>
       <c r="D114" t="n">
-        <v>-12998.05086326599</v>
+        <v>-12998.04047203064</v>
       </c>
       <c r="E114" t="n">
-        <v>-12.99805086326599</v>
+        <v>-12.99804047203064</v>
       </c>
     </row>
     <row r="115">
@@ -2631,13 +2631,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>88531.3144197464</v>
+        <v>88531.23874282837</v>
       </c>
       <c r="D116" t="n">
-        <v>-11468.6855802536</v>
+        <v>-11468.76125717163</v>
       </c>
       <c r="E116" t="n">
-        <v>-11.4686855802536</v>
+        <v>-11.46876125717163</v>
       </c>
     </row>
     <row r="117">
@@ -2688,13 +2688,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>84247.34219741821</v>
+        <v>84247.30129623413</v>
       </c>
       <c r="D119" t="n">
-        <v>-15752.65780258179</v>
+        <v>-15752.69870376587</v>
       </c>
       <c r="E119" t="n">
-        <v>-15.75265780258179</v>
+        <v>-15.75269870376587</v>
       </c>
     </row>
     <row r="120">
@@ -2726,13 +2726,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>114163.7169709206</v>
+        <v>114163.7407717705</v>
       </c>
       <c r="D121" t="n">
-        <v>14163.71697092056</v>
+        <v>14163.74077177048</v>
       </c>
       <c r="E121" t="n">
-        <v>14.16371697092056</v>
+        <v>14.16374077177048</v>
       </c>
     </row>
     <row r="122">
@@ -2779,17 +2779,17 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>brk-b</t>
+          <t>blk</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>111270.224319458</v>
+        <v>114590.0794067383</v>
       </c>
       <c r="D124" t="n">
-        <v>11270.22431945801</v>
+        <v>14590.07940673828</v>
       </c>
       <c r="E124" t="n">
-        <v>11.27022431945801</v>
+        <v>14.59007940673828</v>
       </c>
     </row>
     <row r="125">
@@ -2798,17 +2798,17 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>blk</t>
+          <t>cb</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>114590.0382080078</v>
+        <v>121326.3487548828</v>
       </c>
       <c r="D125" t="n">
-        <v>14590.03820800781</v>
+        <v>21326.34875488281</v>
       </c>
       <c r="E125" t="n">
-        <v>14.59003820800781</v>
+        <v>21.32634875488281</v>
       </c>
     </row>
     <row r="126">
@@ -2817,17 +2817,17 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>cb</t>
+          <t>clf</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>121326.219039917</v>
+        <v>76151.9315662384</v>
       </c>
       <c r="D126" t="n">
-        <v>21326.21903991699</v>
+        <v>-23848.0684337616</v>
       </c>
       <c r="E126" t="n">
-        <v>21.32621903991699</v>
+        <v>-23.8480684337616</v>
       </c>
     </row>
     <row r="127">
@@ -2836,17 +2836,17 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>clf</t>
+          <t>cnx</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>76151.9315662384</v>
+        <v>69128.5512342453</v>
       </c>
       <c r="D127" t="n">
-        <v>-23848.0684337616</v>
+        <v>-30871.4487657547</v>
       </c>
       <c r="E127" t="n">
-        <v>-23.8480684337616</v>
+        <v>-30.8714487657547</v>
       </c>
     </row>
     <row r="128">
@@ -2855,17 +2855,17 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>cnx</t>
+          <t>dv</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>69128.5512342453</v>
+        <v>101120.9239883423</v>
       </c>
       <c r="D128" t="n">
-        <v>-30871.4487657547</v>
+        <v>1120.923988342285</v>
       </c>
       <c r="E128" t="n">
-        <v>-30.8714487657547</v>
+        <v>1.120923988342285</v>
       </c>
     </row>
     <row r="129">
@@ -2874,17 +2874,17 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>dv</t>
+          <t>fhn</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>101120.9239883423</v>
+        <v>97843.06047821045</v>
       </c>
       <c r="D129" t="n">
-        <v>1120.923988342285</v>
+        <v>-2156.939521789551</v>
       </c>
       <c r="E129" t="n">
-        <v>1.120923988342285</v>
+        <v>-2.156939521789551</v>
       </c>
     </row>
     <row r="130">
@@ -2893,17 +2893,17 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>fhn</t>
+          <t>fslr</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>97842.93194389343</v>
+        <v>108201.1974716187</v>
       </c>
       <c r="D130" t="n">
-        <v>-2157.068056106567</v>
+        <v>8201.197471618652</v>
       </c>
       <c r="E130" t="n">
-        <v>-2.157068056106568</v>
+        <v>8.201197471618652</v>
       </c>
     </row>
     <row r="131">
@@ -2912,17 +2912,17 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>fslr</t>
+          <t>flr</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>108201.1974716187</v>
+        <v>67688.45340919495</v>
       </c>
       <c r="D131" t="n">
-        <v>8201.197471618652</v>
+        <v>-32311.54659080505</v>
       </c>
       <c r="E131" t="n">
-        <v>8.201197471618652</v>
+        <v>-32.31154659080505</v>
       </c>
     </row>
     <row r="132">
@@ -2931,17 +2931,17 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>flr</t>
+          <t>fosl</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>67688.45340919495</v>
+        <v>61098.62028884888</v>
       </c>
       <c r="D132" t="n">
-        <v>-32311.54659080505</v>
+        <v>-38901.37971115112</v>
       </c>
       <c r="E132" t="n">
-        <v>-32.31154659080505</v>
+        <v>-38.90137971115112</v>
       </c>
     </row>
     <row r="133">
@@ -2950,17 +2950,17 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>fosl</t>
+          <t>gme</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>61098.62028884888</v>
+        <v>231896.5905952454</v>
       </c>
       <c r="D133" t="n">
-        <v>-38901.37971115112</v>
+        <v>131896.5905952454</v>
       </c>
       <c r="E133" t="n">
-        <v>-38.90137971115112</v>
+        <v>131.8965905952454</v>
       </c>
     </row>
     <row r="134">
@@ -2969,17 +2969,17 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>gme</t>
+          <t>gci</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>231896.5905952454</v>
+        <v>100525.0842018127</v>
       </c>
       <c r="D134" t="n">
-        <v>131896.5905952454</v>
+        <v>525.0842018127441</v>
       </c>
       <c r="E134" t="n">
-        <v>131.8965905952454</v>
+        <v>0.5250842018127442</v>
       </c>
     </row>
     <row r="135">
@@ -2988,17 +2988,17 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>gci</t>
+          <t>gnw</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>100525.0842018127</v>
+        <v>112915.426718235</v>
       </c>
       <c r="D135" t="n">
-        <v>525.0842018127441</v>
+        <v>12915.42671823502</v>
       </c>
       <c r="E135" t="n">
-        <v>0.5250842018127442</v>
+        <v>12.91542671823501</v>
       </c>
     </row>
     <row r="136">
@@ -3007,17 +3007,17 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>gnw</t>
+          <t>gt</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>112915.426718235</v>
+        <v>99834.12429904938</v>
       </c>
       <c r="D136" t="n">
-        <v>12915.42671823502</v>
+        <v>-165.8757009506226</v>
       </c>
       <c r="E136" t="n">
-        <v>12.91542671823501</v>
+        <v>-0.1658757009506225</v>
       </c>
     </row>
     <row r="137">
@@ -3026,17 +3026,17 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>hal</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>99834.12429904938</v>
+        <v>98376.82267951965</v>
       </c>
       <c r="D137" t="n">
-        <v>-165.8757009506226</v>
+        <v>-1623.177320480347</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.1658757009506225</v>
+        <v>-1.623177320480347</v>
       </c>
     </row>
     <row r="138">
@@ -3045,17 +3045,17 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>hal</t>
+          <t>hog</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>98376.63759422302</v>
+        <v>99655.72766494751</v>
       </c>
       <c r="D138" t="n">
-        <v>-1623.362405776978</v>
+        <v>-344.2723350524902</v>
       </c>
       <c r="E138" t="n">
-        <v>-1.623362405776977</v>
+        <v>-0.3442723350524902</v>
       </c>
     </row>
     <row r="139">
@@ -3064,17 +3064,17 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>hog</t>
+          <t>hp</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>99655.79009246826</v>
+        <v>106387.6657276154</v>
       </c>
       <c r="D139" t="n">
-        <v>-344.2099075317383</v>
+        <v>6387.665727615356</v>
       </c>
       <c r="E139" t="n">
-        <v>-0.3442099075317382</v>
+        <v>6.387665727615357</v>
       </c>
     </row>
     <row r="140">
@@ -3083,17 +3083,17 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>hp</t>
+          <t>itw</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>106387.635723114</v>
+        <v>121379.5389251709</v>
       </c>
       <c r="D140" t="n">
-        <v>6387.635723114014</v>
+        <v>21379.5389251709</v>
       </c>
       <c r="E140" t="n">
-        <v>6.387635723114014</v>
+        <v>21.3795389251709</v>
       </c>
     </row>
     <row r="141">
@@ -3102,17 +3102,17 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>itw</t>
+          <t>ice</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>121379.5859375</v>
+        <v>107016.5471725464</v>
       </c>
       <c r="D141" t="n">
-        <v>21379.5859375</v>
+        <v>7016.547172546387</v>
       </c>
       <c r="E141" t="n">
-        <v>21.3795859375</v>
+        <v>7.016547172546386</v>
       </c>
     </row>
     <row r="142">
@@ -3121,17 +3121,17 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>ice</t>
+          <t>igt</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>107016.5700302124</v>
+        <v>122012.6050271988</v>
       </c>
       <c r="D142" t="n">
-        <v>7016.570030212402</v>
+        <v>22012.60502719879</v>
       </c>
       <c r="E142" t="n">
-        <v>7.016570030212402</v>
+        <v>22.01260502719879</v>
       </c>
     </row>
     <row r="143">
@@ -3140,17 +3140,17 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>igt</t>
+          <t>tap</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>122012.5880861282</v>
+        <v>89891.62728500366</v>
       </c>
       <c r="D143" t="n">
-        <v>22012.58808612823</v>
+        <v>-10108.37271499634</v>
       </c>
       <c r="E143" t="n">
-        <v>22.01258808612824</v>
+        <v>-10.10837271499634</v>
       </c>
     </row>
     <row r="144">
@@ -3159,17 +3159,17 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>tap</t>
+          <t>mur</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>89891.6614112854</v>
+        <v>123955.0852737427</v>
       </c>
       <c r="D144" t="n">
-        <v>-10108.3385887146</v>
+        <v>23955.08527374268</v>
       </c>
       <c r="E144" t="n">
-        <v>-10.1083385887146</v>
+        <v>23.95508527374268</v>
       </c>
     </row>
     <row r="145">
@@ -3178,36 +3178,17 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>mur</t>
+          <t>rrc</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>123955.0502548218</v>
+        <v>160804.6068000793</v>
       </c>
       <c r="D145" t="n">
-        <v>23955.05025482178</v>
+        <v>60804.60680007935</v>
       </c>
       <c r="E145" t="n">
-        <v>23.95505025482178</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>rrc</t>
-        </is>
-      </c>
-      <c r="C146" t="n">
-        <v>160804.5859537125</v>
-      </c>
-      <c r="D146" t="n">
-        <v>60804.58595371246</v>
-      </c>
-      <c r="E146" t="n">
-        <v>60.80458595371246</v>
+        <v>60.80460680007934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>